<commit_message>
add fabric io and fixed handlebars
</commit_message>
<xml_diff>
--- a/lavahound-node-server/hunts/Hunts.xlsx
+++ b/lavahound-node-server/hunts/Hunts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25280" windowHeight="15360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="174">
-  <si>
-    <t>Photo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="220">
   <si>
     <t>Message</t>
   </si>
@@ -512,9 +509,6 @@
     <t>Parkway</t>
   </si>
   <si>
-    <t>Use Photo</t>
-  </si>
-  <si>
     <t>MerchantExchange.jpg</t>
   </si>
   <si>
@@ -543,6 +537,151 @@
   </si>
   <si>
     <t>Nice work, feel free to buy Ben Franklin a beer for his influence on Philadelphia</t>
+  </si>
+  <si>
+    <t>Franklin Head</t>
+  </si>
+  <si>
+    <t>Ben Franklin invented the lightning rod, odometer, swim fins, bifocals, and the skullet.</t>
+  </si>
+  <si>
+    <t>While you're here, see if you can find the portrait of Ben Franklin.</t>
+  </si>
+  <si>
+    <t>Franklin Stereo</t>
+  </si>
+  <si>
+    <t>While living in England, Ben Franklin invented a phonetic alphabet. Sir Mix-a-Lot was never formally knighted by the Queen.</t>
+  </si>
+  <si>
+    <t>Franklin Institute Statue</t>
+  </si>
+  <si>
+    <t>Ben Franklin earned the title of "The First American" for his early and indefatigable campaigning for colonial unity.</t>
+  </si>
+  <si>
+    <t>Franklin Head 2</t>
+  </si>
+  <si>
+    <t>Ben Franklin played the guitar, harp, and violin. He also invented an improved version of the armonica.</t>
+  </si>
+  <si>
+    <t>Vine Street</t>
+  </si>
+  <si>
+    <t>Ben Franklin was the first known chess player in the colonies. He was inducted into the U.S. Chess Hall of Fame in 1999.</t>
+  </si>
+  <si>
+    <t>Penn Park Bench</t>
+  </si>
+  <si>
+    <t>Ben Franklin was the first U.S. Postmaster General and published the first political cartoon in the U.S.</t>
+  </si>
+  <si>
+    <t>Grab a seat next to Ben. He's very polite and charming.</t>
+  </si>
+  <si>
+    <t>Founders Hall</t>
+  </si>
+  <si>
+    <t>Ben Franklin founded the University of Pennsylvania. He proposed the nation's first modern liberal arts curriculum.</t>
+  </si>
+  <si>
+    <t>Parkway Ben</t>
+  </si>
+  <si>
+    <t>Ben Franklin enjoyed the warm embrace of a fellow patriot.</t>
+  </si>
+  <si>
+    <t>Gelato Ben</t>
+  </si>
+  <si>
+    <t>Benjamin Franklin had a fervent distaste for tyranny and a strong preference for strawberry gelato.</t>
+  </si>
+  <si>
+    <t>The Ben Franklin Hotel</t>
+  </si>
+  <si>
+    <t>"A penny saved is a penny earned." --Ben Franklin</t>
+  </si>
+  <si>
+    <t>Washington Square</t>
+  </si>
+  <si>
+    <t>Ben Franklin invented many social conventions such as pay it forward.</t>
+  </si>
+  <si>
+    <t>Pay it forward. Do a kind deed for a stranger in honor of Ben.</t>
+  </si>
+  <si>
+    <t>Fire Marshall Franklin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben Franklin formed both the first fire deparment and the first public lending library in America.
+</t>
+  </si>
+  <si>
+    <t>Ben Franklin - Craftsman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ben Franklin was a leading author, printer, postmaster, scientist, musician, inventor, satirist, statesman, and diplomat. </t>
+  </si>
+  <si>
+    <t>Split Wall Image</t>
+  </si>
+  <si>
+    <t>Ben Franklin has been on the American $100 bill since 1928.</t>
+  </si>
+  <si>
+    <t>Christ Church was the final resting place for Ben Franklin.</t>
+  </si>
+  <si>
+    <t>Where is Ben</t>
+  </si>
+  <si>
+    <t>Photo Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>CHALLENGE: Leaving a penny on Franklin's grave is a Philadelphia tradition. Feel free to give it a try.</t>
+  </si>
+  <si>
+    <t>Benjamin_Franklin_National_Memorial.jpg</t>
+  </si>
+  <si>
+    <t>benfhat.jpg</t>
+  </si>
+  <si>
+    <t>Benjamin_Franklin_on_a_Bench.jpg</t>
+  </si>
+  <si>
+    <t>bigben3.jpg</t>
+  </si>
+  <si>
+    <t>Benjamin_Franklin_statue_in_front_of_College_Hall.JPG</t>
+  </si>
+  <si>
+    <t>christ-church-burial.jpg</t>
+  </si>
+  <si>
+    <t>PSU-Philadelphia-Liberty-Trail-Franklin-Key-statue-Michael-Milne-768x1024.jpg</t>
+  </si>
+  <si>
+    <t>ss_060725_philly_02.ss_full.jpg</t>
+  </si>
+  <si>
+    <t>Young_Franklin.jpg</t>
+  </si>
+  <si>
+    <t>39.950691, -75.143807</t>
+  </si>
+  <si>
+    <t>39.958224, -75.172662</t>
+  </si>
+  <si>
+    <t>39.954197, -75.165681</t>
   </si>
 </sst>
 </file>
@@ -625,8 +764,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="125">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -759,7 +924,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="125">
+  <cellStyles count="151">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -822,6 +987,19 @@
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -884,6 +1062,19 @@
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1183,10 +1374,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1201,45 +1393,48 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" t="str">
         <f>CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D2,"','",B2,"','",E2,"','",F2,"', 10, ",C2,");")</f>
@@ -1252,22 +1447,22 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G8" si="0">CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D3,"','",B3,"','",E3,"','",F3,"', 10, ",C3,");")</f>
@@ -1280,22 +1475,22 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -1308,22 +1503,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -1336,22 +1531,22 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -1364,22 +1559,22 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -1392,22 +1587,22 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -1420,91 +1615,91 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="3" customFormat="1"/>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
         <v>55</v>
       </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" t="s">
         <v>72</v>
-      </c>
-      <c r="F14" t="s">
-        <v>73</v>
       </c>
       <c r="G14" t="str">
         <f>CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D14,"','",B14,"','",E14,"','",F14,"', 10, ",C14,");")</f>
@@ -1517,22 +1712,22 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>68</v>
-      </c>
-      <c r="F15" t="s">
-        <v>69</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" ref="G15:G24" si="2">CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D15,"','",B15,"','",E15,"','",F15,"', 10, ",C15,");")</f>
@@ -1545,22 +1740,22 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="2"/>
@@ -1573,22 +1768,22 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="2"/>
@@ -1601,22 +1796,22 @@
     </row>
     <row r="18" spans="1:8" ht="16">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F18" t="s">
         <v>171</v>
-      </c>
-      <c r="F18" t="s">
-        <v>173</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="2"/>
@@ -1629,19 +1824,19 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" t="s">
         <v>91</v>
-      </c>
-      <c r="F19" t="s">
-        <v>92</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="2"/>
@@ -1654,19 +1849,19 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" t="s">
         <v>93</v>
-      </c>
-      <c r="F20" t="s">
-        <v>94</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="2"/>
@@ -1679,19 +1874,19 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" t="s">
         <v>95</v>
-      </c>
-      <c r="F21" t="s">
-        <v>96</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="2"/>
@@ -1704,19 +1899,19 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" t="s">
         <v>97</v>
-      </c>
-      <c r="F22" t="s">
-        <v>98</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="2"/>
@@ -1729,19 +1924,19 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
         <v>99</v>
-      </c>
-      <c r="F23" t="s">
-        <v>100</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="2"/>
@@ -1754,19 +1949,19 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="2"/>
@@ -1780,21 +1975,23 @@
     <row r="25" spans="1:8" s="3" customFormat="1"/>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E26" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>103</v>
-      </c>
-      <c r="F26" t="s">
-        <v>104</v>
       </c>
       <c r="G26" t="str">
         <f>CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D26,"','",B26,"','",E26,"','",F26,"', 10, ",C26,");")</f>
-        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'','The Love Statue','One of several variations of Robert Indiana's Iconic "LOVE" Statue, this one was gifted to the University of Pennsylvania by Jeffrey and Silvia Loria in 1998. Another version of the statue exists in Philadelphia's LOVE Park (or JFK Plaza).','"LOVE" can also be found in places like NYC, Kansas, Utah, Japan, China, and Kytgzstan. There is also a version showing the word in Italian (AMOR) in Milan, and one in Hebew (AHAVA) in Jerusalem.', 10, );</v>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'','The Love Statue','One of several variations of Robert Indiana's Iconic "LOVE" Statue, this one was gifted to the University of Pennsylvania by Jeffrey and Silvia Loria in 1998. Another version of the statue exists in Philadelphia's LOVE Park (or JFK Plaza).','"LOVE" can also be found in places like NYC, Kansas, Utah, Japan, China, and Kytgzstan. There is also a version showing the word in Italian (AMOR) in Milan, and one in Hebew (AHAVA) in Jerusalem.', 10, 39.954197, -75.165681);</v>
       </c>
       <c r="H26" t="str">
         <f>CONCATENATE("insert into hunt_photo select photo_id, 4 from photo where title = '",B26,"';")</f>
@@ -1803,17 +2000,17 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1"/>
       <c r="E27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" t="s">
         <v>106</v>
-      </c>
-      <c r="F27" t="s">
-        <v>107</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" ref="G27:G35" si="4">CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D27,"','",B27,"','",E27,"','",F27,"', 10, ",C27,");")</f>
@@ -1826,17 +2023,17 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28" s="1"/>
       <c r="E28" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" t="s">
         <v>109</v>
-      </c>
-      <c r="F28" t="s">
-        <v>110</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="4"/>
@@ -1849,17 +2046,17 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29" s="1"/>
       <c r="E29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" t="s">
         <v>112</v>
-      </c>
-      <c r="F29" t="s">
-        <v>113</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="4"/>
@@ -1872,17 +2069,17 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" s="1"/>
       <c r="E30" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" t="s">
         <v>115</v>
-      </c>
-      <c r="F30" t="s">
-        <v>116</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="4"/>
@@ -1895,17 +2092,17 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31" s="1"/>
       <c r="E31" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" t="s">
         <v>118</v>
-      </c>
-      <c r="F31" t="s">
-        <v>119</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="4"/>
@@ -1918,17 +2115,17 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32" s="1"/>
       <c r="E32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" t="s">
         <v>121</v>
-      </c>
-      <c r="F32" t="s">
-        <v>122</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="4"/>
@@ -1941,17 +2138,17 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="1"/>
       <c r="E33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" t="s">
         <v>124</v>
-      </c>
-      <c r="F33" t="s">
-        <v>125</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="4"/>
@@ -1964,17 +2161,17 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C34" s="1"/>
       <c r="E34" t="s">
+        <v>126</v>
+      </c>
+      <c r="F34" t="s">
         <v>127</v>
-      </c>
-      <c r="F34" t="s">
-        <v>128</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="4"/>
@@ -1987,17 +2184,17 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C35" s="1"/>
       <c r="E35" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" t="s">
         <v>130</v>
-      </c>
-      <c r="F35" t="s">
-        <v>131</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="4"/>
@@ -2011,23 +2208,21 @@
     <row r="36" spans="1:8" s="3" customFormat="1"/>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>163</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C37" s="1"/>
       <c r="E37" t="s">
+        <v>132</v>
+      </c>
+      <c r="F37" t="s">
         <v>133</v>
-      </c>
-      <c r="F37" t="s">
-        <v>134</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" ref="G37" si="6">CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D37,"','",B37,"','",E37,"','",F37,"', 10, ",C37,");")</f>
-        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'','Rocky Statue','Rocky was filmed on a budget of less than $1 million. It made $275 million and won the Oscar for Best Picture in 1976.   ','There are no statues of Thunderlips or George Washington Duke.', 10, Use Photo);</v>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'','Rocky Statue','Rocky was filmed on a budget of less than $1 million. It made $275 million and won the Oscar for Best Picture in 1976.   ','There are no statues of Thunderlips or George Washington Duke.', 10, );</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("insert into hunt_photo select photo_id, 5 from photo where title = '",B37,"';")</f>
@@ -2036,23 +2231,21 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>163</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C38" s="1"/>
       <c r="E38" t="s">
+        <v>134</v>
+      </c>
+      <c r="F38" t="s">
         <v>135</v>
-      </c>
-      <c r="F38" t="s">
-        <v>136</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" ref="G38:G48" si="7">CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D38,"','",B38,"','",E38,"','",F38,"', 10, ",C38,");")</f>
-        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'','Rocky Steps','There are 72 Rocky Steps. The steps appear in every film in the series except Rocky IV.','Challenge: Rocky ran up the steps in 10.2 seconds. See if you can beat his time. ', 10, Use Photo);</v>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'','Rocky Steps','There are 72 Rocky Steps. The steps appear in every film in the series except Rocky IV.','Challenge: Rocky ran up the steps in 10.2 seconds. See if you can beat his time. ', 10, );</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" ref="H38:H48" si="8">CONCATENATE("insert into hunt_photo select photo_id, 5 from photo where title = '",B38,"';")</f>
@@ -2061,17 +2254,17 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C39" s="1"/>
       <c r="E39" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" t="s">
         <v>138</v>
-      </c>
-      <c r="F39" t="s">
-        <v>139</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="7"/>
@@ -2084,17 +2277,17 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C40" s="1"/>
       <c r="E40" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" t="s">
         <v>141</v>
-      </c>
-      <c r="F40" t="s">
-        <v>142</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="7"/>
@@ -2107,14 +2300,14 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C41" s="1"/>
       <c r="E41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="7"/>
@@ -2127,14 +2320,14 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C42" s="1"/>
       <c r="E42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="7"/>
@@ -2147,17 +2340,17 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C43" s="1"/>
       <c r="E43" t="s">
+        <v>147</v>
+      </c>
+      <c r="F43" t="s">
         <v>148</v>
-      </c>
-      <c r="F43" t="s">
-        <v>149</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="7"/>
@@ -2170,14 +2363,14 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C44" s="1"/>
       <c r="E44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="7"/>
@@ -2190,17 +2383,17 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C45" s="1"/>
       <c r="E45" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" t="s">
         <v>153</v>
-      </c>
-      <c r="F45" t="s">
-        <v>154</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="7"/>
@@ -2213,14 +2406,14 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C46" s="1"/>
       <c r="E46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="7"/>
@@ -2233,14 +2426,14 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C47" s="1"/>
       <c r="E47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="7"/>
@@ -2253,17 +2446,17 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B48" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C48" s="1"/>
       <c r="E48" t="s">
+        <v>159</v>
+      </c>
+      <c r="F48" t="s">
         <v>160</v>
-      </c>
-      <c r="F48" t="s">
-        <v>161</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="7"/>
@@ -2274,45 +2467,309 @@
         <v>insert into hunt_photo select photo_id, 5 from photo where title = 'Turtle';</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+    <row r="49" spans="1:8" s="3" customFormat="1"/>
+    <row r="50" spans="1:8">
+      <c r="A50" t="s">
+        <v>164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>165</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B51" t="s">
-        <v>167</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+    </row>
+    <row r="51" spans="1:8" s="3" customFormat="1"/>
+    <row r="52" spans="1:8">
+      <c r="A52" t="s">
+        <v>204</v>
+      </c>
+      <c r="B52" t="s">
+        <v>197</v>
+      </c>
       <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D52" t="s">
+        <v>209</v>
+      </c>
+      <c r="E52" t="s">
+        <v>198</v>
+      </c>
+      <c r="G52" t="str">
+        <f t="shared" ref="G52" si="9">CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D52,"','",B52,"','",E52,"','",F52,"', 10, ",C52,");")</f>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'benfhat.jpg','Fire Marshall Franklin','Ben Franklin formed both the first fire deparment and the first public lending library in America._x000D__x000D_','', 10, );</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" ref="H52" si="10">CONCATENATE("insert into hunt_photo select photo_id, 5 from photo where title = '",B52,"';")</f>
+        <v>insert into hunt_photo select photo_id, 5 from photo where title = 'Fire Marshall Franklin';</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" t="s">
+        <v>204</v>
+      </c>
+      <c r="B53" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D53" t="s">
+        <v>208</v>
+      </c>
+      <c r="E53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G53" t="str">
+        <f t="shared" ref="G53:G58" si="11">CONCATENATE("insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'", D53,"','",B53,"','",E53,"','",F53,"', 10, ",C53,");")</f>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'Benjamin_Franklin_National_Memorial.jpg','Franklin Institute Statue','Ben Franklin earned the title of "The First American" for his early and indefatigable campaigning for colonial unity.','', 10, 39.958224, -75.172662);</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" ref="H53:H58" si="12">CONCATENATE("insert into hunt_photo select photo_id, 5 from photo where title = '",B53,"';")</f>
+        <v>insert into hunt_photo select photo_id, 5 from photo where title = 'Franklin Institute Statue';</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" t="s">
+        <v>183</v>
+      </c>
       <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" t="s">
+        <v>210</v>
+      </c>
+      <c r="E54" t="s">
+        <v>184</v>
+      </c>
+      <c r="F54" t="s">
+        <v>185</v>
+      </c>
+      <c r="G54" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'Benjamin_Franklin_on_a_Bench.jpg','Penn Park Bench','Ben Franklin was the first U.S. Postmaster General and published the first political cartoon in the U.S.','Grab a seat next to Ben. He's very polite and charming.', 10, );</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into hunt_photo select photo_id, 5 from photo where title = 'Penn Park Bench';</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55" t="s">
+        <v>186</v>
+      </c>
       <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D55" t="s">
+        <v>212</v>
+      </c>
+      <c r="E55" t="s">
+        <v>187</v>
+      </c>
+      <c r="F55" t="s">
+        <v>148</v>
+      </c>
+      <c r="G55" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'Benjamin_Franklin_statue_in_front_of_College_Hall.JPG','Founders Hall','Ben Franklin founded the University of Pennsylvania. He proposed the nation's first modern liberal arts curriculum.','.', 10, );</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into hunt_photo select photo_id, 5 from photo where title = 'Founders Hall';</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="16">
+      <c r="A56" t="s">
+        <v>204</v>
+      </c>
+      <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D56" t="s">
+        <v>213</v>
+      </c>
+      <c r="E56" t="s">
+        <v>203</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="G56" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'christ-church-burial.jpg','Christ Church','Christ Church was the final resting place for Ben Franklin.','CHALLENGE: Leaving a penny on Franklin's grave is a Philadelphia tradition. Feel free to give it a try.', 10, 39.950691, -75.143807);</v>
+      </c>
+      <c r="H56" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into hunt_photo select photo_id, 5 from photo where title = 'Christ Church';</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" t="s">
+        <v>204</v>
+      </c>
+      <c r="B57" t="s">
+        <v>172</v>
+      </c>
       <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57" t="s">
+        <v>214</v>
+      </c>
+      <c r="E57" t="s">
+        <v>173</v>
+      </c>
+      <c r="F57" t="s">
+        <v>174</v>
+      </c>
+      <c r="G57" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'PSU-Philadelphia-Liberty-Trail-Franklin-Key-statue-Michael-Milne-768x1024.jpg','Franklin Head','Ben Franklin invented the lightning rod, odometer, swim fins, bifocals, and the skullet.','While you're here, see if you can find the portrait of Ben Franklin.', 10, );</v>
+      </c>
+      <c r="H57" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into hunt_photo select photo_id, 5 from photo where title = 'Franklin Head';</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" t="s">
+        <v>204</v>
+      </c>
+      <c r="B58" t="s">
+        <v>199</v>
+      </c>
       <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58" t="s">
+        <v>215</v>
+      </c>
+      <c r="E58" t="s">
+        <v>200</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into photo(photo_id, account_id, image_file_name, title, description,found_msg, points, latitude, longitude) values(nextval('photo_id_seq'),1,'ss_060725_philly_02.ss_full.jpg','Ben Franklin - Craftsman','Ben Franklin was a leading author, printer, postmaster, scientist, musician, inventor, satirist, statesman, and diplomat. ','', 10, );</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" si="12"/>
+        <v>insert into hunt_photo select photo_id, 5 from photo where title = 'Ben Franklin - Craftsman';</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" t="s">
+        <v>204</v>
+      </c>
+      <c r="B59" t="s">
+        <v>175</v>
+      </c>
       <c r="C59" s="1"/>
+      <c r="E59" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B60" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="E60" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" t="s">
+        <v>204</v>
+      </c>
+      <c r="B61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="E61" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" t="s">
+        <v>204</v>
+      </c>
+      <c r="B62" t="s">
+        <v>188</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="E62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" t="s">
+        <v>204</v>
+      </c>
+      <c r="B63" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="E63" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" t="s">
+        <v>204</v>
+      </c>
+      <c r="B64" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="E64" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" t="s">
+        <v>194</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="E65" t="s">
+        <v>195</v>
+      </c>
+      <c r="F65" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>204</v>
+      </c>
+      <c r="B66" t="s">
+        <v>201</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="E66" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="E69" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="E70" t="s">
+        <v>211</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A52:F66">
+    <sortCondition ref="D52:D66"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>

</xml_diff>